<commit_message>
ajout fichier session 2
</commit_message>
<xml_diff>
--- a/tableau-exel.xlsx
+++ b/tableau-exel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ned\Desktop\travail-nader-gouasmi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ned\Desktop\nader_gouasmi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{611A7249-4C3B-4F89-81FD-637285E9021F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2841D7E-0E58-4624-B1F9-FD72D2861493}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{2F473DE1-3555-4B30-8BFB-271864F594FA}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
   <si>
     <t>mardi</t>
   </si>
@@ -57,9 +57,6 @@
     <t>la page navigation</t>
   </si>
   <si>
-    <t>la page a propos de moi</t>
-  </si>
-  <si>
     <t>des exemples de portfolio</t>
   </si>
   <si>
@@ -79,6 +76,33 @@
   </si>
   <si>
     <t>BD:en cours</t>
+  </si>
+  <si>
+    <t>la page home</t>
+  </si>
+  <si>
+    <t>la partie responsive du site</t>
+  </si>
+  <si>
+    <t>//</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lundi </t>
+  </si>
+  <si>
+    <t>mise en forme des bouttons</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jeudi </t>
+  </si>
+  <si>
+    <t>la page login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la page sign up </t>
+  </si>
+  <si>
+    <t>mise en forme du site avec jquery</t>
   </si>
 </sst>
 </file>
@@ -430,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E972DB-9502-4674-9221-BACA67E1478A}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,7 +487,7 @@
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -471,10 +495,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -482,10 +506,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -493,13 +517,54 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>